<commit_message>
relatorio geral exportando em excel detalhado
</commit_message>
<xml_diff>
--- a/src/resources/net/gnfe/excel/relatorio-geral.xlsx
+++ b/src/resources/net/gnfe/excel/relatorio-geral.xlsx
@@ -5,35 +5,90 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IdeaProjects\projeto-tcc\src\resources\net\gnfe\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guial\IdeaProjects\gnfe\src\resources\net\gnfe\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF5F912-2A59-4E8D-B3B4-F8C33677C815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7FAB4C-95D9-4F24-85FF-CB58FF4C70B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Requisições" sheetId="1" r:id="rId1"/>
+    <sheet name="Movimentações" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>ID Movimentação Produto</t>
+  </si>
+  <si>
+    <t>ID Orçamento</t>
+  </si>
+  <si>
+    <t>ID Nota Fiscal</t>
+  </si>
+  <si>
+    <t>ID Produto</t>
+  </si>
+  <si>
+    <t>Forma de Pagamento</t>
+  </si>
+  <si>
+    <t>Bandeira</t>
+  </si>
+  <si>
+    <t>Nome do Produto</t>
+  </si>
+  <si>
+    <t>Data de Cancelamento Nota Fiscal</t>
+  </si>
+  <si>
+    <t>Data de Envio Nota Fiscal</t>
+  </si>
+  <si>
+    <t>Status da Nota Fiscal</t>
+  </si>
+  <si>
+    <t>Data de Criação Nota Fiscal</t>
+  </si>
+  <si>
+    <t>Nome do Cliente</t>
+  </si>
+  <si>
+    <t>Nome do Autor</t>
+  </si>
+  <si>
+    <t>Chave de Acesso Nota Fiscal</t>
+  </si>
+  <si>
+    <t>Protocolo de Envio Nota Fiscal</t>
+  </si>
+  <si>
+    <t>Protocolo de Cancelamento Nota Fiscal</t>
+  </si>
+  <si>
+    <t>Valor da Unidade do Produto</t>
+  </si>
+  <si>
+    <t>Estoque Atual do Produto</t>
+  </si>
+  <si>
+    <t>Motivo da Movimentação</t>
+  </si>
+  <si>
+    <t>Tipo de Movimentação</t>
+  </si>
+  <si>
+    <t>Estoque Atual da Movimentação</t>
+  </si>
+  <si>
+    <t>Valor Total da Movimentação</t>
+  </si>
+  <si>
+    <t>Data da Movimentação</t>
   </si>
 </sst>
 </file>
@@ -57,12 +112,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -92,9 +153,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,31 +437,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.42578125" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" customWidth="1"/>
+    <col min="17" max="17" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24" customWidth="1"/>
+    <col min="20" max="20" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
inclusão de valor de compra e ajuste no relatório
</commit_message>
<xml_diff>
--- a/src/resources/net/gnfe/excel/relatorio-geral.xlsx
+++ b/src/resources/net/gnfe/excel/relatorio-geral.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guial\IdeaProjects\gnfe\src\resources\net\gnfe\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A7FAB4C-95D9-4F24-85FF-CB58FF4C70B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0684D6-2ECE-4EC3-99DC-9312E1293605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Movimentações" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ID Movimentação Produto</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>Data da Movimentação</t>
+  </si>
+  <si>
+    <t>Hora da Movimentação</t>
+  </si>
+  <si>
+    <t>Valor de Compra Unidade do Produto</t>
   </si>
 </sst>
 </file>
@@ -437,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,17 +465,17 @@
     <col min="13" max="13" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.7109375" customWidth="1"/>
-    <col min="17" max="17" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24" customWidth="1"/>
-    <col min="20" max="20" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="30.7109375" customWidth="1"/>
+    <col min="18" max="18" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="24" customWidth="1"/>
+    <col min="22" max="22" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,21 +528,27 @@
         <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>